<commit_message>
Final calibration before sharing
</commit_message>
<xml_diff>
--- a/data/static/input/parameters.xlsx
+++ b/data/static/input/parameters.xlsx
@@ -1,21 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2ae90f5cbd0fd171/UVA/Thesis/MSc-Thesis/data/static/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adenooy/Library/CloudStorage/OneDrive-Personal/UVA/Thesis/MSc-Thesis/data/static/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="346" documentId="8_{0B355B81-4B94-8A4D-8227-7AC0012709BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A107F514-3A0D-1245-B422-9FB196C0FEFD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9172590-73BD-5E49-9CE8-8F3E887CC01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{52823E06-76C8-E540-A826-14346C881C14}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="3" xr2:uid="{52823E06-76C8-E540-A826-14346C881C14}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="3" r:id="rId1"/>
-    <sheet name="kenya" sheetId="4" r:id="rId2"/>
+    <sheet name="baseline" sheetId="4" r:id="rId2"/>
+    <sheet name="scenario1" sheetId="5" r:id="rId3"/>
+    <sheet name="parameter changes" sheetId="8" r:id="rId4"/>
+    <sheet name="scenario2" sheetId="6" r:id="rId5"/>
+    <sheet name="scenario3" sheetId="7" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">scenario1!$A$1:$G$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">scenario2!$A$1:$G$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">scenario3!$A$1:$F$47</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="59">
   <si>
     <t>prev</t>
   </si>
@@ -190,6 +199,30 @@
   </si>
   <si>
     <t>time_sample_testing</t>
+  </si>
+  <si>
+    <t>no match</t>
+  </si>
+  <si>
+    <t>Scen 3</t>
+  </si>
+  <si>
+    <t>scen 2</t>
+  </si>
+  <si>
+    <t>scen 1</t>
+  </si>
+  <si>
+    <t>Scenario 1</t>
+  </si>
+  <si>
+    <t>Scenario 2</t>
+  </si>
+  <si>
+    <t>Scenario 3</t>
+  </si>
+  <si>
+    <t>baseline</t>
   </si>
 </sst>
 </file>
@@ -477,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -513,6 +546,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1648,10 +1682,836 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4375ED64-D1A0-0D46-98F2-0651DCD3DE97}">
+  <dimension ref="A1:G47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="25"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7">
+        <v>7.9044417396061259E-2</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.25093200581395353</v>
+      </c>
+      <c r="D2" s="17">
+        <v>9.9989059080962794E-3</v>
+      </c>
+      <c r="E2" s="10">
+        <v>3.7337209000000003E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="D3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="E3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.13</v>
+      </c>
+      <c r="C4">
+        <v>0.13</v>
+      </c>
+      <c r="D4">
+        <v>0.13</v>
+      </c>
+      <c r="E4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>0.84</v>
+      </c>
+      <c r="C15">
+        <v>0.84</v>
+      </c>
+      <c r="D15">
+        <v>0.84</v>
+      </c>
+      <c r="E15">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <f>1-0.53</f>
+        <v>0.47</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:E17" si="0">1-0.53</f>
+        <v>0.47</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0.47</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="C19">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="D19">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="E19">
+        <v>0.53100000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="21">
+        <v>0.85</v>
+      </c>
+      <c r="C20" s="22">
+        <v>0.81</v>
+      </c>
+      <c r="D20">
+        <v>0.82</v>
+      </c>
+      <c r="E20">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="19">
+        <v>0.98</v>
+      </c>
+      <c r="C21" s="20">
+        <v>0.98</v>
+      </c>
+      <c r="D21">
+        <v>0.89</v>
+      </c>
+      <c r="E21">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="C22">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="D22">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="E22">
+        <v>0.46899999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="12">
+        <v>0.68</v>
+      </c>
+      <c r="C23" s="13">
+        <v>0.52</v>
+      </c>
+      <c r="D23" s="13">
+        <v>0.4</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="C24" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="D24" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="E24" s="23">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="C28" s="23">
+        <v>0.19</v>
+      </c>
+      <c r="D28" s="23">
+        <v>1</v>
+      </c>
+      <c r="E28" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <f>1-0.67</f>
+        <v>0.32999999999999996</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30:E30" si="1">1-0.67</f>
+        <v>0.32999999999999996</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>0.32999999999999996</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>0.32999999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="C31" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="D31" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="E31" s="12">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="12">
+        <v>0.92</v>
+      </c>
+      <c r="C33" s="12">
+        <v>0.92</v>
+      </c>
+      <c r="D33" s="12">
+        <v>0.92</v>
+      </c>
+      <c r="E33" s="12">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <v>0.31</v>
+      </c>
+      <c r="C35">
+        <v>0.31</v>
+      </c>
+      <c r="D35">
+        <v>0.31</v>
+      </c>
+      <c r="E35">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="18">
+        <v>1</v>
+      </c>
+      <c r="C36" s="18">
+        <v>1</v>
+      </c>
+      <c r="D36" s="18">
+        <v>1</v>
+      </c>
+      <c r="E36" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="18">
+        <v>1</v>
+      </c>
+      <c r="C37" s="18">
+        <v>1</v>
+      </c>
+      <c r="D37" s="18">
+        <v>1</v>
+      </c>
+      <c r="E37" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="18">
+        <v>1</v>
+      </c>
+      <c r="C38" s="18">
+        <v>1</v>
+      </c>
+      <c r="D38" s="18">
+        <v>1</v>
+      </c>
+      <c r="E38" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="18">
+        <v>1</v>
+      </c>
+      <c r="C39" s="18">
+        <v>1</v>
+      </c>
+      <c r="D39" s="18">
+        <v>1</v>
+      </c>
+      <c r="E39" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="18">
+        <v>1</v>
+      </c>
+      <c r="C40" s="18">
+        <v>1</v>
+      </c>
+      <c r="D40" s="18">
+        <v>1</v>
+      </c>
+      <c r="E40" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="18">
+        <v>1</v>
+      </c>
+      <c r="C41" s="18">
+        <v>1</v>
+      </c>
+      <c r="D41" s="18">
+        <v>1</v>
+      </c>
+      <c r="E41" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="18">
+        <v>1</v>
+      </c>
+      <c r="C42" s="18">
+        <v>1</v>
+      </c>
+      <c r="D42" s="18">
+        <v>1</v>
+      </c>
+      <c r="E42" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="18">
+        <v>1</v>
+      </c>
+      <c r="C43" s="18">
+        <v>1</v>
+      </c>
+      <c r="D43" s="18">
+        <v>1</v>
+      </c>
+      <c r="E43" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="18">
+        <v>1</v>
+      </c>
+      <c r="C44" s="18">
+        <v>1</v>
+      </c>
+      <c r="D44" s="18">
+        <v>1</v>
+      </c>
+      <c r="E44" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45" s="18">
+        <v>1</v>
+      </c>
+      <c r="C45" s="18">
+        <v>1</v>
+      </c>
+      <c r="D45" s="18">
+        <v>1</v>
+      </c>
+      <c r="E45" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="18">
+        <v>1</v>
+      </c>
+      <c r="C46" s="18">
+        <v>1</v>
+      </c>
+      <c r="D46" s="18">
+        <v>1</v>
+      </c>
+      <c r="E46" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="18">
+        <v>1</v>
+      </c>
+      <c r="C47" s="18">
+        <v>1</v>
+      </c>
+      <c r="D47" s="18">
+        <v>1</v>
+      </c>
+      <c r="E47" s="18">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113B92D8-4B08-3948-96E4-452C348CA2EA}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1974,16 +2834,16 @@
         <v>15</v>
       </c>
       <c r="B19">
-        <v>0.53100000000000003</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>0.53100000000000003</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>0.53100000000000003</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>0.53100000000000003</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2025,16 +2885,16 @@
         <v>18</v>
       </c>
       <c r="B22">
-        <v>0.46899999999999997</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>0.46899999999999997</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>0.46899999999999997</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>0.46899999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -2175,6 +3035,1990 @@
       <c r="E30">
         <f t="shared" si="1"/>
         <v>0.32999999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="C31" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="D31" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="E31" s="12">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="12">
+        <v>0.92</v>
+      </c>
+      <c r="C33" s="12">
+        <v>0.92</v>
+      </c>
+      <c r="D33" s="12">
+        <v>0.92</v>
+      </c>
+      <c r="E33" s="12">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <v>0.31</v>
+      </c>
+      <c r="C35">
+        <v>0.31</v>
+      </c>
+      <c r="D35">
+        <v>0.31</v>
+      </c>
+      <c r="E35">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="18">
+        <v>1</v>
+      </c>
+      <c r="C36" s="18">
+        <v>1</v>
+      </c>
+      <c r="D36" s="18">
+        <v>1</v>
+      </c>
+      <c r="E36" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="18">
+        <v>1</v>
+      </c>
+      <c r="C37" s="18">
+        <v>1</v>
+      </c>
+      <c r="D37" s="18">
+        <v>1</v>
+      </c>
+      <c r="E37" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="18">
+        <v>1</v>
+      </c>
+      <c r="C38" s="18">
+        <v>1</v>
+      </c>
+      <c r="D38" s="18">
+        <v>1</v>
+      </c>
+      <c r="E38" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="18">
+        <v>1</v>
+      </c>
+      <c r="C39" s="18">
+        <v>1</v>
+      </c>
+      <c r="D39" s="18">
+        <v>1</v>
+      </c>
+      <c r="E39" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="18">
+        <v>1</v>
+      </c>
+      <c r="C40" s="18">
+        <v>1</v>
+      </c>
+      <c r="D40" s="18">
+        <v>1</v>
+      </c>
+      <c r="E40" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="18">
+        <v>1</v>
+      </c>
+      <c r="C41" s="18">
+        <v>1</v>
+      </c>
+      <c r="D41" s="18">
+        <v>1</v>
+      </c>
+      <c r="E41" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="18">
+        <v>1</v>
+      </c>
+      <c r="C42" s="18">
+        <v>1</v>
+      </c>
+      <c r="D42" s="18">
+        <v>1</v>
+      </c>
+      <c r="E42" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="18">
+        <v>1</v>
+      </c>
+      <c r="C43" s="18">
+        <v>1</v>
+      </c>
+      <c r="D43" s="18">
+        <v>1</v>
+      </c>
+      <c r="E43" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="18">
+        <v>1</v>
+      </c>
+      <c r="C44" s="18">
+        <v>1</v>
+      </c>
+      <c r="D44" s="18">
+        <v>1</v>
+      </c>
+      <c r="E44" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45" s="18">
+        <v>1</v>
+      </c>
+      <c r="C45" s="18">
+        <v>1</v>
+      </c>
+      <c r="D45" s="18">
+        <v>1</v>
+      </c>
+      <c r="E45" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="18">
+        <v>1</v>
+      </c>
+      <c r="C46" s="18">
+        <v>1</v>
+      </c>
+      <c r="D46" s="18">
+        <v>1</v>
+      </c>
+      <c r="E46" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="18">
+        <v>1</v>
+      </c>
+      <c r="C47" s="18">
+        <v>1</v>
+      </c>
+      <c r="D47" s="18">
+        <v>1</v>
+      </c>
+      <c r="E47" s="18">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143E317C-B13E-F149-9322-DDFB1391BCEC}">
+  <dimension ref="A2:H28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9746A4DB-C09F-E84C-AFAF-DDB3D67C1B9B}">
+  <dimension ref="A1:E47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7">
+        <v>7.9044417396061259E-2</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.25093200581395353</v>
+      </c>
+      <c r="D2" s="17">
+        <v>9.9989059080962794E-3</v>
+      </c>
+      <c r="E2" s="10">
+        <v>3.7337209000000003E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="D3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="E3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.13</v>
+      </c>
+      <c r="C4">
+        <v>0.13</v>
+      </c>
+      <c r="D4">
+        <v>0.13</v>
+      </c>
+      <c r="E4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>0.84</v>
+      </c>
+      <c r="C15">
+        <v>0.84</v>
+      </c>
+      <c r="D15">
+        <v>0.84</v>
+      </c>
+      <c r="E15">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <f>1-0.53</f>
+        <v>0.47</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:E17" si="0">1-0.53</f>
+        <v>0.47</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0.47</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="21">
+        <v>0.85</v>
+      </c>
+      <c r="C20" s="22">
+        <v>0.81</v>
+      </c>
+      <c r="D20">
+        <v>0.82</v>
+      </c>
+      <c r="E20">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="19">
+        <v>0.98</v>
+      </c>
+      <c r="C21" s="20">
+        <v>0.98</v>
+      </c>
+      <c r="D21">
+        <v>0.89</v>
+      </c>
+      <c r="E21">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="12">
+        <v>0.68</v>
+      </c>
+      <c r="C23" s="13">
+        <v>0.52</v>
+      </c>
+      <c r="D23" s="13">
+        <v>0.4</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="C24" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="D24" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="E24" s="23">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="C28" s="23">
+        <v>0.19</v>
+      </c>
+      <c r="D28" s="23">
+        <v>1</v>
+      </c>
+      <c r="E28" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="C31" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="D31" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="E31" s="12">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="12">
+        <v>0.92</v>
+      </c>
+      <c r="C33" s="12">
+        <v>0.92</v>
+      </c>
+      <c r="D33" s="12">
+        <v>0.92</v>
+      </c>
+      <c r="E33" s="12">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <v>0.31</v>
+      </c>
+      <c r="C35">
+        <v>0.31</v>
+      </c>
+      <c r="D35">
+        <v>0.31</v>
+      </c>
+      <c r="E35">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="18">
+        <v>1</v>
+      </c>
+      <c r="C36" s="18">
+        <v>1</v>
+      </c>
+      <c r="D36" s="18">
+        <v>1</v>
+      </c>
+      <c r="E36" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="18">
+        <v>1</v>
+      </c>
+      <c r="C37" s="18">
+        <v>1</v>
+      </c>
+      <c r="D37" s="18">
+        <v>1</v>
+      </c>
+      <c r="E37" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="18">
+        <v>1</v>
+      </c>
+      <c r="C38" s="18">
+        <v>1</v>
+      </c>
+      <c r="D38" s="18">
+        <v>1</v>
+      </c>
+      <c r="E38" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="18">
+        <v>1</v>
+      </c>
+      <c r="C39" s="18">
+        <v>1</v>
+      </c>
+      <c r="D39" s="18">
+        <v>1</v>
+      </c>
+      <c r="E39" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="18">
+        <v>1</v>
+      </c>
+      <c r="C40" s="18">
+        <v>1</v>
+      </c>
+      <c r="D40" s="18">
+        <v>1</v>
+      </c>
+      <c r="E40" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="18">
+        <v>1</v>
+      </c>
+      <c r="C41" s="18">
+        <v>1</v>
+      </c>
+      <c r="D41" s="18">
+        <v>1</v>
+      </c>
+      <c r="E41" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="18">
+        <v>1</v>
+      </c>
+      <c r="C42" s="18">
+        <v>1</v>
+      </c>
+      <c r="D42" s="18">
+        <v>1</v>
+      </c>
+      <c r="E42" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="18">
+        <v>1</v>
+      </c>
+      <c r="C43" s="18">
+        <v>1</v>
+      </c>
+      <c r="D43" s="18">
+        <v>1</v>
+      </c>
+      <c r="E43" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="18">
+        <v>1</v>
+      </c>
+      <c r="C44" s="18">
+        <v>1</v>
+      </c>
+      <c r="D44" s="18">
+        <v>1</v>
+      </c>
+      <c r="E44" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45" s="18">
+        <v>1</v>
+      </c>
+      <c r="C45" s="18">
+        <v>1</v>
+      </c>
+      <c r="D45" s="18">
+        <v>1</v>
+      </c>
+      <c r="E45" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="18">
+        <v>1</v>
+      </c>
+      <c r="C46" s="18">
+        <v>1</v>
+      </c>
+      <c r="D46" s="18">
+        <v>1</v>
+      </c>
+      <c r="E46" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="18">
+        <v>1</v>
+      </c>
+      <c r="C47" s="18">
+        <v>1</v>
+      </c>
+      <c r="D47" s="18">
+        <v>1</v>
+      </c>
+      <c r="E47" s="18">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BD4BA19-5F99-034E-B1D4-C7699EAD05D1}">
+  <dimension ref="A1:E47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7">
+        <v>7.9044417396061259E-2</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.25093200581395353</v>
+      </c>
+      <c r="D2" s="17">
+        <v>9.9989059080962794E-3</v>
+      </c>
+      <c r="E2" s="10">
+        <v>3.7337209000000003E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="D3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="E3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.13</v>
+      </c>
+      <c r="C4">
+        <v>0.13</v>
+      </c>
+      <c r="D4">
+        <v>0.13</v>
+      </c>
+      <c r="E4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>0.84</v>
+      </c>
+      <c r="C15">
+        <v>0.84</v>
+      </c>
+      <c r="D15">
+        <v>0.84</v>
+      </c>
+      <c r="E15">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="21">
+        <v>0.85</v>
+      </c>
+      <c r="C20" s="22">
+        <v>0.81</v>
+      </c>
+      <c r="D20">
+        <v>0.82</v>
+      </c>
+      <c r="E20">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="19">
+        <v>0.98</v>
+      </c>
+      <c r="C21" s="20">
+        <v>0.98</v>
+      </c>
+      <c r="D21">
+        <v>0.89</v>
+      </c>
+      <c r="E21">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="12">
+        <v>0.68</v>
+      </c>
+      <c r="C23" s="13">
+        <v>0.52</v>
+      </c>
+      <c r="D23" s="13">
+        <v>0.4</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="C24" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="D24" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="E24" s="23">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="C28" s="23">
+        <v>0.19</v>
+      </c>
+      <c r="D28" s="23">
+        <v>1</v>
+      </c>
+      <c r="E28" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
New static scenarios, dynamic equlibirum and exp 1
</commit_message>
<xml_diff>
--- a/data/static/input/parameters.xlsx
+++ b/data/static/input/parameters.xlsx
@@ -1,29 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adenooy/Library/CloudStorage/OneDrive-Personal/UVA/Thesis/MSc-Thesis/data/static/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9172590-73BD-5E49-9CE8-8F3E887CC01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE2B451-7E3B-2F42-85E6-466040709C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="3" xr2:uid="{52823E06-76C8-E540-A826-14346C881C14}"/>
+    <workbookView xWindow="-2620" yWindow="-19060" windowWidth="28800" windowHeight="16100" activeTab="8" xr2:uid="{52823E06-76C8-E540-A826-14346C881C14}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="3" r:id="rId1"/>
     <sheet name="baseline" sheetId="4" r:id="rId2"/>
     <sheet name="scenario1" sheetId="5" r:id="rId3"/>
-    <sheet name="parameter changes" sheetId="8" r:id="rId4"/>
-    <sheet name="scenario2" sheetId="6" r:id="rId5"/>
-    <sheet name="scenario3" sheetId="7" r:id="rId6"/>
+    <sheet name="scenario2" sheetId="6" r:id="rId4"/>
+    <sheet name="scenario3" sheetId="7" r:id="rId5"/>
+    <sheet name="parameter changes" sheetId="8" r:id="rId6"/>
+    <sheet name="scenario4" sheetId="9" r:id="rId7"/>
+    <sheet name="scenario5" sheetId="11" r:id="rId8"/>
+    <sheet name="scenario6" sheetId="12" r:id="rId9"/>
+    <sheet name="Sheet2" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">scenario1!$A$1:$G$47</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">scenario2!$A$1:$G$47</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">scenario3!$A$1:$F$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">scenario2!$A$1:$G$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">scenario3!$A$1:$F$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">scenario4!$A$1:$G$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">scenario5!$A$1:$G$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">scenario6!$A$1:$F$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="69">
   <si>
     <t>prev</t>
   </si>
@@ -201,9 +208,6 @@
     <t>time_sample_testing</t>
   </si>
   <si>
-    <t>no match</t>
-  </si>
-  <si>
     <t>Scen 3</t>
   </si>
   <si>
@@ -223,6 +227,39 @@
   </si>
   <si>
     <t>baseline</t>
+  </si>
+  <si>
+    <t>sputum</t>
+  </si>
+  <si>
+    <t>non-sputum</t>
+  </si>
+  <si>
+    <t>scen4</t>
+  </si>
+  <si>
+    <t>swab</t>
+  </si>
+  <si>
+    <t>p_no_sample *</t>
+  </si>
+  <si>
+    <t>xpert accuracy **</t>
+  </si>
+  <si>
+    <t>** Swabs only affect Xpert accuracy in cases which are not extrapulmonary TB</t>
+  </si>
+  <si>
+    <t>Scenario 4</t>
+  </si>
+  <si>
+    <t>Scenario 5</t>
+  </si>
+  <si>
+    <t>Scenario 6</t>
+  </si>
+  <si>
+    <t>* The use of swab only affects those without extrapulmonary TB as more invasive samples are required for this diagnosis is all cases</t>
   </si>
 </sst>
 </file>
@@ -301,7 +338,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -506,11 +543,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -546,7 +607,26 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1680,12 +1760,124 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A996B1F9-29CC-D540-AB86-6D69A30CD911}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C1" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="21">
+        <v>0.91</v>
+      </c>
+      <c r="D2" s="22">
+        <v>0.9</v>
+      </c>
+      <c r="E2">
+        <v>0.82</v>
+      </c>
+      <c r="F2">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="19">
+        <v>0.96</v>
+      </c>
+      <c r="D3" s="20">
+        <v>0.96</v>
+      </c>
+      <c r="E3">
+        <v>0.89</v>
+      </c>
+      <c r="F3">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="D4">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="E4">
+        <v>0.82</v>
+      </c>
+      <c r="F4">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="16">
+        <v>0.96</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0.96</v>
+      </c>
+      <c r="E5">
+        <v>0.89</v>
+      </c>
+      <c r="F5">
+        <v>0.89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4375ED64-D1A0-0D46-98F2-0651DCD3DE97}">
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B15" sqref="B15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1937,16 +2129,16 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
       <c r="C15">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
       <c r="D15">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
       <c r="E15">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -2026,10 +2218,10 @@
         <v>16</v>
       </c>
       <c r="B20" s="21">
-        <v>0.85</v>
+        <v>0.91</v>
       </c>
       <c r="C20" s="22">
-        <v>0.81</v>
+        <v>0.9</v>
       </c>
       <c r="D20">
         <v>0.82</v>
@@ -2043,10 +2235,10 @@
         <v>17</v>
       </c>
       <c r="B21" s="19">
-        <v>0.98</v>
+        <v>0.96</v>
       </c>
       <c r="C21" s="20">
-        <v>0.98</v>
+        <v>0.96</v>
       </c>
       <c r="D21">
         <v>0.89</v>
@@ -2511,7 +2703,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="B15" sqref="B15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2762,16 +2954,16 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
       <c r="C15">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
       <c r="D15">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
       <c r="E15">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -2851,10 +3043,10 @@
         <v>16</v>
       </c>
       <c r="B20" s="21">
-        <v>0.85</v>
+        <v>0.91</v>
       </c>
       <c r="C20" s="22">
-        <v>0.81</v>
+        <v>0.9</v>
       </c>
       <c r="D20">
         <v>0.82</v>
@@ -3332,354 +3524,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143E317C-B13E-F149-9322-DDFB1391BCEC}">
-  <dimension ref="A2:H28"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11" s="25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H18" s="25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9746A4DB-C09F-E84C-AFAF-DDB3D67C1B9B}">
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="B15" sqref="B15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3930,16 +3779,16 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
       <c r="C15">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
       <c r="D15">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
       <c r="E15">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -4019,10 +3868,10 @@
         <v>16</v>
       </c>
       <c r="B20" s="21">
-        <v>0.85</v>
+        <v>0.91</v>
       </c>
       <c r="C20" s="22">
-        <v>0.81</v>
+        <v>0.9</v>
       </c>
       <c r="D20">
         <v>0.82</v>
@@ -4495,12 +4344,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BD4BA19-5F99-034E-B1D4-C7699EAD05D1}">
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="B15" sqref="B15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4754,16 +4603,16 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
       <c r="C15">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
       <c r="D15">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
       <c r="E15">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -4839,10 +4688,10 @@
         <v>16</v>
       </c>
       <c r="B20" s="21">
-        <v>0.85</v>
+        <v>0.91</v>
       </c>
       <c r="C20" s="22">
-        <v>0.81</v>
+        <v>0.9</v>
       </c>
       <c r="D20">
         <v>0.82</v>
@@ -4979,6 +4828,3081 @@
       </c>
       <c r="C28" s="23">
         <v>0.19</v>
+      </c>
+      <c r="D28" s="23">
+        <v>1</v>
+      </c>
+      <c r="E28" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="C31" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="D31" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="E31" s="12">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="12">
+        <v>0.92</v>
+      </c>
+      <c r="C33" s="12">
+        <v>0.92</v>
+      </c>
+      <c r="D33" s="12">
+        <v>0.92</v>
+      </c>
+      <c r="E33" s="12">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <v>0.31</v>
+      </c>
+      <c r="C35">
+        <v>0.31</v>
+      </c>
+      <c r="D35">
+        <v>0.31</v>
+      </c>
+      <c r="E35">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="18">
+        <v>1</v>
+      </c>
+      <c r="C36" s="18">
+        <v>1</v>
+      </c>
+      <c r="D36" s="18">
+        <v>1</v>
+      </c>
+      <c r="E36" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="18">
+        <v>1</v>
+      </c>
+      <c r="C37" s="18">
+        <v>1</v>
+      </c>
+      <c r="D37" s="18">
+        <v>1</v>
+      </c>
+      <c r="E37" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="18">
+        <v>1</v>
+      </c>
+      <c r="C38" s="18">
+        <v>1</v>
+      </c>
+      <c r="D38" s="18">
+        <v>1</v>
+      </c>
+      <c r="E38" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="18">
+        <v>1</v>
+      </c>
+      <c r="C39" s="18">
+        <v>1</v>
+      </c>
+      <c r="D39" s="18">
+        <v>1</v>
+      </c>
+      <c r="E39" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="18">
+        <v>1</v>
+      </c>
+      <c r="C40" s="18">
+        <v>1</v>
+      </c>
+      <c r="D40" s="18">
+        <v>1</v>
+      </c>
+      <c r="E40" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="18">
+        <v>1</v>
+      </c>
+      <c r="C41" s="18">
+        <v>1</v>
+      </c>
+      <c r="D41" s="18">
+        <v>1</v>
+      </c>
+      <c r="E41" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="18">
+        <v>1</v>
+      </c>
+      <c r="C42" s="18">
+        <v>1</v>
+      </c>
+      <c r="D42" s="18">
+        <v>1</v>
+      </c>
+      <c r="E42" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="18">
+        <v>1</v>
+      </c>
+      <c r="C43" s="18">
+        <v>1</v>
+      </c>
+      <c r="D43" s="18">
+        <v>1</v>
+      </c>
+      <c r="E43" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="18">
+        <v>1</v>
+      </c>
+      <c r="C44" s="18">
+        <v>1</v>
+      </c>
+      <c r="D44" s="18">
+        <v>1</v>
+      </c>
+      <c r="E44" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45" s="18">
+        <v>1</v>
+      </c>
+      <c r="C45" s="18">
+        <v>1</v>
+      </c>
+      <c r="D45" s="18">
+        <v>1</v>
+      </c>
+      <c r="E45" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="18">
+        <v>1</v>
+      </c>
+      <c r="C46" s="18">
+        <v>1</v>
+      </c>
+      <c r="D46" s="18">
+        <v>1</v>
+      </c>
+      <c r="E46" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="18">
+        <v>1</v>
+      </c>
+      <c r="C47" s="18">
+        <v>1</v>
+      </c>
+      <c r="D47" s="18">
+        <v>1</v>
+      </c>
+      <c r="E47" s="18">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143E317C-B13E-F149-9322-DDFB1391BCEC}">
+  <dimension ref="A2:R33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.33203125" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="N4" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="O4" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="P4" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q4" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="R4" s="27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="O5" s="13">
+        <v>0</v>
+      </c>
+      <c r="P5" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q5" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="R5" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="13">
+        <v>1</v>
+      </c>
+      <c r="N6" s="13">
+        <v>1</v>
+      </c>
+      <c r="O6" s="13">
+        <v>1</v>
+      </c>
+      <c r="P6" s="13">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="13">
+        <v>1</v>
+      </c>
+      <c r="R6" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="13">
+        <v>0</v>
+      </c>
+      <c r="N7" s="13">
+        <v>0</v>
+      </c>
+      <c r="O7" s="13">
+        <v>0</v>
+      </c>
+      <c r="P7" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="13">
+        <v>0</v>
+      </c>
+      <c r="R7" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="26">
+        <v>0.85</v>
+      </c>
+      <c r="C8" s="26">
+        <v>0.81</v>
+      </c>
+      <c r="D8">
+        <v>0.82</v>
+      </c>
+      <c r="E8">
+        <v>0.82</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="N8" s="13">
+        <v>0</v>
+      </c>
+      <c r="O8" s="13">
+        <v>0</v>
+      </c>
+      <c r="P8" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q8" s="13">
+        <v>0</v>
+      </c>
+      <c r="R8" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="26">
+        <v>0.98</v>
+      </c>
+      <c r="C9" s="26">
+        <v>0.98</v>
+      </c>
+      <c r="D9">
+        <v>0.89</v>
+      </c>
+      <c r="E9">
+        <v>0.89</v>
+      </c>
+      <c r="L9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="N9" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="O9" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="P9" s="28">
+        <v>0.95</v>
+      </c>
+      <c r="Q9" s="28">
+        <v>0.95</v>
+      </c>
+      <c r="R9" s="13">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="L10" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="O10" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="P10" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="28">
+        <v>0</v>
+      </c>
+      <c r="R10" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="L11" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="N11" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="O11" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="P11" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q11" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="R11" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L12" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="L13" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="32"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="26">
+        <v>0.85</v>
+      </c>
+      <c r="C17" s="26">
+        <v>0.81</v>
+      </c>
+      <c r="D17">
+        <v>0.82</v>
+      </c>
+      <c r="E17">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="26">
+        <v>0.98</v>
+      </c>
+      <c r="C18" s="26">
+        <v>0.98</v>
+      </c>
+      <c r="D18">
+        <v>0.89</v>
+      </c>
+      <c r="E18">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="23">
+        <v>0</v>
+      </c>
+      <c r="C30" s="23">
+        <v>0</v>
+      </c>
+      <c r="D30" s="23">
+        <v>1</v>
+      </c>
+      <c r="E30" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="G32" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32">
+        <v>0.95</v>
+      </c>
+      <c r="I32">
+        <v>0.95</v>
+      </c>
+      <c r="J32">
+        <v>0.95</v>
+      </c>
+      <c r="K32">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="L12:R12"/>
+    <mergeCell ref="L13:R13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAEA5E35-7A77-A342-95DE-41D724A79E0F}">
+  <dimension ref="A1:E47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7">
+        <v>7.9044417396061259E-2</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.25093200581395353</v>
+      </c>
+      <c r="D2" s="17">
+        <v>9.9989059080962794E-3</v>
+      </c>
+      <c r="E2" s="10">
+        <v>3.7337209000000003E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="D3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="E3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.13</v>
+      </c>
+      <c r="C4">
+        <v>0.13</v>
+      </c>
+      <c r="D4">
+        <v>0.13</v>
+      </c>
+      <c r="E4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>0.9</v>
+      </c>
+      <c r="C15">
+        <v>0.9</v>
+      </c>
+      <c r="D15">
+        <v>0.9</v>
+      </c>
+      <c r="E15">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <f>1-0.53</f>
+        <v>0.47</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:E17" si="0">1-0.53</f>
+        <v>0.47</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0.47</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="C20">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="D20">
+        <v>0.82</v>
+      </c>
+      <c r="E20">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="19">
+        <v>0.98</v>
+      </c>
+      <c r="C21" s="20">
+        <v>0.98</v>
+      </c>
+      <c r="D21">
+        <v>0.89</v>
+      </c>
+      <c r="E21">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="12">
+        <v>0.68</v>
+      </c>
+      <c r="C23" s="13">
+        <v>0.52</v>
+      </c>
+      <c r="D23" s="13">
+        <v>0.4</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="C24" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="D24" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="E24" s="23">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="23">
+        <v>0</v>
+      </c>
+      <c r="C28" s="23">
+        <v>0</v>
+      </c>
+      <c r="D28" s="23">
+        <v>1</v>
+      </c>
+      <c r="E28" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <f>1-0.67</f>
+        <v>0.32999999999999996</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30:E30" si="1">1-0.67</f>
+        <v>0.32999999999999996</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>0.32999999999999996</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>0.32999999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="C31" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="D31" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="E31" s="12">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="12">
+        <v>0.92</v>
+      </c>
+      <c r="C33" s="12">
+        <v>0.92</v>
+      </c>
+      <c r="D33" s="12">
+        <v>0.92</v>
+      </c>
+      <c r="E33" s="12">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <v>0.31</v>
+      </c>
+      <c r="C35">
+        <v>0.31</v>
+      </c>
+      <c r="D35">
+        <v>0.31</v>
+      </c>
+      <c r="E35">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="18">
+        <v>1</v>
+      </c>
+      <c r="C36" s="18">
+        <v>1</v>
+      </c>
+      <c r="D36" s="18">
+        <v>1</v>
+      </c>
+      <c r="E36" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="18">
+        <v>1</v>
+      </c>
+      <c r="C37" s="18">
+        <v>1</v>
+      </c>
+      <c r="D37" s="18">
+        <v>1</v>
+      </c>
+      <c r="E37" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="18">
+        <v>1</v>
+      </c>
+      <c r="C38" s="18">
+        <v>1</v>
+      </c>
+      <c r="D38" s="18">
+        <v>1</v>
+      </c>
+      <c r="E38" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="18">
+        <v>1</v>
+      </c>
+      <c r="C39" s="18">
+        <v>1</v>
+      </c>
+      <c r="D39" s="18">
+        <v>1</v>
+      </c>
+      <c r="E39" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="18">
+        <v>1</v>
+      </c>
+      <c r="C40" s="18">
+        <v>1</v>
+      </c>
+      <c r="D40" s="18">
+        <v>1</v>
+      </c>
+      <c r="E40" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="18">
+        <v>1</v>
+      </c>
+      <c r="C41" s="18">
+        <v>1</v>
+      </c>
+      <c r="D41" s="18">
+        <v>1</v>
+      </c>
+      <c r="E41" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="18">
+        <v>1</v>
+      </c>
+      <c r="C42" s="18">
+        <v>1</v>
+      </c>
+      <c r="D42" s="18">
+        <v>1</v>
+      </c>
+      <c r="E42" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="18">
+        <v>1</v>
+      </c>
+      <c r="C43" s="18">
+        <v>1</v>
+      </c>
+      <c r="D43" s="18">
+        <v>1</v>
+      </c>
+      <c r="E43" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="18">
+        <v>1</v>
+      </c>
+      <c r="C44" s="18">
+        <v>1</v>
+      </c>
+      <c r="D44" s="18">
+        <v>1</v>
+      </c>
+      <c r="E44" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45" s="18">
+        <v>1</v>
+      </c>
+      <c r="C45" s="18">
+        <v>1</v>
+      </c>
+      <c r="D45" s="18">
+        <v>1</v>
+      </c>
+      <c r="E45" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="18">
+        <v>1</v>
+      </c>
+      <c r="C46" s="18">
+        <v>1</v>
+      </c>
+      <c r="D46" s="18">
+        <v>1</v>
+      </c>
+      <c r="E46" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="18">
+        <v>1</v>
+      </c>
+      <c r="C47" s="18">
+        <v>1</v>
+      </c>
+      <c r="D47" s="18">
+        <v>1</v>
+      </c>
+      <c r="E47" s="18">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C025E5F8-03BD-6E44-A109-56D051FB8833}">
+  <dimension ref="A1:E47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7">
+        <v>7.9044417396061259E-2</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.25093200581395353</v>
+      </c>
+      <c r="D2" s="17">
+        <v>9.9989059080962794E-3</v>
+      </c>
+      <c r="E2" s="10">
+        <v>3.7337209000000003E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="D3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="E3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.13</v>
+      </c>
+      <c r="C4">
+        <v>0.13</v>
+      </c>
+      <c r="D4">
+        <v>0.13</v>
+      </c>
+      <c r="E4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>0.9</v>
+      </c>
+      <c r="C15">
+        <v>0.9</v>
+      </c>
+      <c r="D15">
+        <v>0.9</v>
+      </c>
+      <c r="E15">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <f>1-0.53</f>
+        <v>0.47</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:E17" si="0">1-0.53</f>
+        <v>0.47</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0.47</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="C20">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="D20">
+        <v>0.82</v>
+      </c>
+      <c r="E20">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="19">
+        <v>0.98</v>
+      </c>
+      <c r="C21" s="20">
+        <v>0.98</v>
+      </c>
+      <c r="D21">
+        <v>0.89</v>
+      </c>
+      <c r="E21">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="12">
+        <v>0.68</v>
+      </c>
+      <c r="C23" s="13">
+        <v>0.52</v>
+      </c>
+      <c r="D23" s="13">
+        <v>0.4</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="C24" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="D24" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="E24" s="23">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="23">
+        <v>0</v>
+      </c>
+      <c r="C28" s="23">
+        <v>0</v>
+      </c>
+      <c r="D28" s="23">
+        <v>1</v>
+      </c>
+      <c r="E28" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="C31" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="D31" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="E31" s="12">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="12">
+        <v>0.92</v>
+      </c>
+      <c r="C33" s="12">
+        <v>0.92</v>
+      </c>
+      <c r="D33" s="12">
+        <v>0.92</v>
+      </c>
+      <c r="E33" s="12">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <v>0.31</v>
+      </c>
+      <c r="C35">
+        <v>0.31</v>
+      </c>
+      <c r="D35">
+        <v>0.31</v>
+      </c>
+      <c r="E35">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="18">
+        <v>1</v>
+      </c>
+      <c r="C36" s="18">
+        <v>1</v>
+      </c>
+      <c r="D36" s="18">
+        <v>1</v>
+      </c>
+      <c r="E36" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="18">
+        <v>1</v>
+      </c>
+      <c r="C37" s="18">
+        <v>1</v>
+      </c>
+      <c r="D37" s="18">
+        <v>1</v>
+      </c>
+      <c r="E37" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="18">
+        <v>1</v>
+      </c>
+      <c r="C38" s="18">
+        <v>1</v>
+      </c>
+      <c r="D38" s="18">
+        <v>1</v>
+      </c>
+      <c r="E38" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="18">
+        <v>1</v>
+      </c>
+      <c r="C39" s="18">
+        <v>1</v>
+      </c>
+      <c r="D39" s="18">
+        <v>1</v>
+      </c>
+      <c r="E39" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="18">
+        <v>1</v>
+      </c>
+      <c r="C40" s="18">
+        <v>1</v>
+      </c>
+      <c r="D40" s="18">
+        <v>1</v>
+      </c>
+      <c r="E40" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="18">
+        <v>1</v>
+      </c>
+      <c r="C41" s="18">
+        <v>1</v>
+      </c>
+      <c r="D41" s="18">
+        <v>1</v>
+      </c>
+      <c r="E41" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="18">
+        <v>1</v>
+      </c>
+      <c r="C42" s="18">
+        <v>1</v>
+      </c>
+      <c r="D42" s="18">
+        <v>1</v>
+      </c>
+      <c r="E42" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="18">
+        <v>1</v>
+      </c>
+      <c r="C43" s="18">
+        <v>1</v>
+      </c>
+      <c r="D43" s="18">
+        <v>1</v>
+      </c>
+      <c r="E43" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="18">
+        <v>1</v>
+      </c>
+      <c r="C44" s="18">
+        <v>1</v>
+      </c>
+      <c r="D44" s="18">
+        <v>1</v>
+      </c>
+      <c r="E44" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45" s="18">
+        <v>1</v>
+      </c>
+      <c r="C45" s="18">
+        <v>1</v>
+      </c>
+      <c r="D45" s="18">
+        <v>1</v>
+      </c>
+      <c r="E45" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="18">
+        <v>1</v>
+      </c>
+      <c r="C46" s="18">
+        <v>1</v>
+      </c>
+      <c r="D46" s="18">
+        <v>1</v>
+      </c>
+      <c r="E46" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="18">
+        <v>1</v>
+      </c>
+      <c r="C47" s="18">
+        <v>1</v>
+      </c>
+      <c r="D47" s="18">
+        <v>1</v>
+      </c>
+      <c r="E47" s="18">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52906AAF-6960-984A-8B48-0C463B67DA01}">
+  <dimension ref="A1:E47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7">
+        <v>7.9044417396061259E-2</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.25093200581395353</v>
+      </c>
+      <c r="D2" s="17">
+        <v>9.9989059080962794E-3</v>
+      </c>
+      <c r="E2" s="10">
+        <v>3.7337209000000003E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="D3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="E3" s="6">
+        <v>8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.13</v>
+      </c>
+      <c r="C4">
+        <v>0.13</v>
+      </c>
+      <c r="D4">
+        <v>0.13</v>
+      </c>
+      <c r="E4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>0.9</v>
+      </c>
+      <c r="C15">
+        <v>0.9</v>
+      </c>
+      <c r="D15">
+        <v>0.9</v>
+      </c>
+      <c r="E15">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="21">
+        <v>0.91</v>
+      </c>
+      <c r="C20" s="22">
+        <v>0.9</v>
+      </c>
+      <c r="D20">
+        <v>0.82</v>
+      </c>
+      <c r="E20">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="19">
+        <v>0.98</v>
+      </c>
+      <c r="C21" s="20">
+        <v>0.98</v>
+      </c>
+      <c r="D21">
+        <v>0.89</v>
+      </c>
+      <c r="E21">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="12">
+        <v>0.68</v>
+      </c>
+      <c r="C23" s="13">
+        <v>0.52</v>
+      </c>
+      <c r="D23" s="13">
+        <v>0.4</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="C24" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="D24" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="E24" s="23">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="23">
+        <v>0</v>
+      </c>
+      <c r="C28" s="23">
+        <v>0</v>
       </c>
       <c r="D28" s="23">
         <v>1</v>

</xml_diff>

<commit_message>
Fix scenario 3 & 6, updated full cohort analysis
</commit_message>
<xml_diff>
--- a/data/static/input/parameters.xlsx
+++ b/data/static/input/parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adenooy/Library/CloudStorage/OneDrive-Personal/UVA/Thesis/MSc-Thesis/data/static/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2ae90f5cbd0fd171/UVA/Thesis/MSc-Thesis/data/static/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EB5300-4A15-494B-B3CA-0A3A7736D981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="6_{073B6C7F-D6B9-3E48-BCDA-A2157B8E6965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{626B5922-4039-E249-BC0E-2E7AE20EEA72}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="-18640" windowWidth="28800" windowHeight="16100" activeTab="4" xr2:uid="{52823E06-76C8-E540-A826-14346C881C14}"/>
+    <workbookView xWindow="40" yWindow="-18640" windowWidth="28800" windowHeight="16100" activeTab="8" xr2:uid="{52823E06-76C8-E540-A826-14346C881C14}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="3" r:id="rId1"/>
@@ -4348,8 +4348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BD4BA19-5F99-034E-B1D4-C7699EAD05D1}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4892,16 +4892,16 @@
         <v>27</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -7423,8 +7423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52906AAF-6960-984A-8B48-0C463B67DA01}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7967,16 +7967,16 @@
         <v>27</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>